<commit_message>
Modul ajar excel template
</commit_message>
<xml_diff>
--- a/public/excel_template/Modul_Ajar_Template.xlsx
+++ b/public/excel_template/Modul_Ajar_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\API-Login-Register\public\excel_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76BCC58-1D0B-4DF7-A994-9738B9E58D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C947A4-C75C-4208-9069-0C733218710E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,6 +345,36 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -365,36 +395,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,8 +616,8 @@
   </sheetPr>
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -632,9 +632,9 @@
     <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -723,15 +723,15 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="28"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -758,15 +758,15 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -795,13 +795,13 @@
     </row>
     <row r="15" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="25"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -811,10 +811,10 @@
       <c r="B16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="39"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -824,10 +824,10 @@
       <c r="B17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="39"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -854,15 +854,15 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="28"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -894,10 +894,10 @@
       <c r="B23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="39"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -929,114 +929,104 @@
       <c r="B26" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="26"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="36"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="32"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="25"/>
     </row>
     <row r="30" spans="1:9" ht="132.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="35"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="28"/>
     </row>
     <row r="31" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="35"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="28"/>
     </row>
     <row r="34" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="35"/>
-    </row>
-    <row r="37" spans="2:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="26"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="28"/>
+    </row>
+    <row r="37" spans="2:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="33"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="35"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="28"/>
     </row>
     <row r="40" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="32"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="25"/>
     </row>
     <row r="41" spans="2:6" ht="249.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="37"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="39"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="32"/>
     </row>
     <row r="46" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="36" t="s">
+      <c r="B46" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="32"/>
-    </row>
-    <row r="47" spans="2:6" ht="132" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="25"/>
+    </row>
+    <row r="47" spans="2:6" ht="167.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C47" s="33"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="35"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="28"/>
     </row>
     <row r="48" spans="2:6" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C48" s="33"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="35"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C37:F37"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="C9:F9"/>
@@ -1046,6 +1036,16 @@
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="C20:F20"/>
     <mergeCell ref="C23:F23"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>